<commit_message>
linearization heuristic is outputting negative controls
</commit_message>
<xml_diff>
--- a/linearization_heuristic_dyn_models/linearization_heuristic_results_60_days.xlsx
+++ b/linearization_heuristic_dyn_models/linearization_heuristic_results_60_days.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,20 +462,30 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>lockdown_freq</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>reward</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>test_freq</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>testing</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>tests</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>xi</t>
         </is>
@@ -486,13 +496,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>47515.31812002748</v>
+        <v>11722.24006150288</v>
       </c>
       <c r="C2" t="n">
         <v>0.5</v>
       </c>
       <c r="D2" t="n">
-        <v>30142648072.11637</v>
+        <v>8954554373.270102</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -500,21 +510,27 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="G2" t="n">
-        <v>24778236975.80526</v>
-      </c>
-      <c r="H2" t="inlineStr">
+        <v>14</v>
+      </c>
+      <c r="H2" t="n">
+        <v>-3831779429.893841</v>
+      </c>
+      <c r="I2" t="n">
+        <v>7</v>
+      </c>
+      <c r="J2" t="inlineStr">
         <is>
           <t>linearization_heuristic</t>
         </is>
       </c>
-      <c r="I2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0</v>
+      <c r="K2" t="n">
+        <v>30000</v>
+      </c>
+      <c r="L2" t="n">
+        <v>1000000</v>
       </c>
     </row>
     <row r="3">
@@ -522,13 +538,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>47901.34001351873</v>
+        <v>9833.931188451937</v>
       </c>
       <c r="C3" t="n">
         <v>0.5</v>
       </c>
       <c r="D3" t="n">
-        <v>30139546356.48362</v>
+        <v>8956426690.199156</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -536,237 +552,27 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="G3" t="n">
-        <v>23304488522.30122</v>
-      </c>
-      <c r="H3" t="inlineStr">
+        <v>14</v>
+      </c>
+      <c r="H3" t="n">
+        <v>-1578617800.467741</v>
+      </c>
+      <c r="I3" t="n">
+        <v>7</v>
+      </c>
+      <c r="J3" t="inlineStr">
         <is>
           <t>linearization_heuristic</t>
         </is>
       </c>
-      <c r="I3" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>51801.90126169195</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="D4" t="n">
-        <v>30139412156.63111</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>linearization_heuristic</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>2000</v>
-      </c>
-      <c r="G4" t="n">
-        <v>24801976584.94373</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>linearization_heuristic</t>
-        </is>
-      </c>
-      <c r="I4" t="n">
+      <c r="K3" t="n">
         <v>30000</v>
       </c>
-      <c r="J4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
-        <v>52212.6801940568</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="D5" t="n">
-        <v>30136109766.00377</v>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>linearization_heuristic_Prop_Bouncing</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
-        <v>2000</v>
-      </c>
-      <c r="G5" t="n">
-        <v>23262018857.74863</v>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>linearization_heuristic</t>
-        </is>
-      </c>
-      <c r="I5" t="n">
-        <v>30000</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>40177.18665674653</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="D6" t="n">
-        <v>23932800629.16895</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>linearization_heuristic</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
-        <v>2000</v>
-      </c>
-      <c r="G6" t="n">
-        <v>-25804015349.88281</v>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>linearization_heuristic</t>
-        </is>
-      </c>
-      <c r="I6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" t="n">
-        <v>1115970.9</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="n">
-        <v>40500.60121923726</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="D7" t="n">
-        <v>23929450317.32204</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>linearization_heuristic_Prop_Bouncing</t>
-        </is>
-      </c>
-      <c r="F7" t="n">
-        <v>2000</v>
-      </c>
-      <c r="G7" t="n">
-        <v>-27106928752.09159</v>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>linearization_heuristic</t>
-        </is>
-      </c>
-      <c r="I7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" t="n">
-        <v>1115970.9</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
-        <v>39996.93753480255</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="D8" t="n">
-        <v>24185932609.20865</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>linearization_heuristic</t>
-        </is>
-      </c>
-      <c r="F8" t="n">
-        <v>2000</v>
-      </c>
-      <c r="G8" t="n">
-        <v>-25365867601.21516</v>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>linearization_heuristic</t>
-        </is>
-      </c>
-      <c r="I8" t="n">
-        <v>30000</v>
-      </c>
-      <c r="J8" t="n">
-        <v>1115970.9</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="n">
-        <v>40319.72706720605</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="D9" t="n">
-        <v>24182605684.08409</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>linearization_heuristic_Prop_Bouncing</t>
-        </is>
-      </c>
-      <c r="F9" t="n">
-        <v>2000</v>
-      </c>
-      <c r="G9" t="n">
-        <v>-26666145727.13618</v>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>linearization_heuristic</t>
-        </is>
-      </c>
-      <c r="I9" t="n">
-        <v>30000</v>
-      </c>
-      <c r="J9" t="n">
-        <v>1115970.9</v>
+      <c r="L3" t="n">
+        <v>1000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>